<commit_message>
Update Inputs and Descriptions in Configs for inputs and outputs
</commit_message>
<xml_diff>
--- a/testing/New_DietData_ISE.xlsx
+++ b/testing/New_DietData_ISE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanryan\Desktop\choice-web\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA73B58E-C47A-426D-9BEE-6A3FB53F5DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979F82B3-FDC5-47A2-89DF-F6011D61574D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="889" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="889" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BackgroundData" sheetId="1" r:id="rId1"/>
@@ -7840,7 +7840,7 @@
   <dimension ref="A1:AB36"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
@@ -10146,13 +10146,13 @@
   <dimension ref="A2:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A10"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
@@ -11962,7 +11962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD04F7E1-2728-4AA0-924E-31014798477C}">
   <dimension ref="A1:T97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
@@ -14502,8 +14502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AS96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31523,7 +31523,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32973,7 +32973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>

</xml_diff>